<commit_message>
Backup: Mon Jan 13 16:59:26 IST 2025
</commit_message>
<xml_diff>
--- a/src/linear_regression_with_significance.xlsx
+++ b/src/linear_regression_with_significance.xlsx
@@ -28,439 +28,439 @@
     <t>P-value</t>
   </si>
   <si>
+    <t>Inferior Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Frontal Medial Cortex Volume Avg</t>
+  </si>
+  <si>
     <t>Temporal Fusiform Cortex, posterior division Change</t>
   </si>
   <si>
+    <t>Superior Parietal Lobule Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Change</t>
+  </si>
+  <si>
     <t>Parahippocampal Gyrus, posterior division Change</t>
   </si>
   <si>
+    <t>Supramarginal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Change</t>
+  </si>
+  <si>
     <t>Superior Temporal Gyrus, posterior division Change</t>
   </si>
   <si>
+    <t>Occipital Fusiform Gyrus Change</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Change</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Change</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Change</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Change</t>
+  </si>
+  <si>
     <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Change</t>
   </si>
   <si>
-    <t>Superior Frontal Gyrus Change</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Change</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Change</t>
+    <t>Middle Temporal Gyrus, posterior division Change</t>
   </si>
   <si>
     <t>Inferior Frontal Gyrus, pars opercularis Change</t>
   </si>
   <si>
-    <t>Postcentral Gyrus Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, posterior division Change</t>
+    <t>Cingulate Gyrus, posterior division Change</t>
   </si>
   <si>
     <t>Temporal Occipital Fusiform Cortex Change</t>
   </si>
   <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Change</t>
+    <t>Frontal Medial Cortex Change</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Change</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Change</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Change</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Change</t>
   </si>
   <si>
     <t>Middle Temporal Gyrus, temporooccipital part Change</t>
   </si>
   <si>
+    <t>Inferior Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Occipital Pole Volume Avg</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus Change</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Change</t>
+  </si>
+  <si>
+    <t>Temporal Pole Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Insular Cortex Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Change</t>
+  </si>
+  <si>
+    <t>Occipital Pole Volume Change</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Planum Polare Volume Avg</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Insular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Volume Avg</t>
+  </si>
+  <si>
+    <t>Insular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Volume Avg</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Planum Temporale Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Volume Avg</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Planum Polare Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Volume Avg</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Volume Change</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Change</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Temporale Volume Avg</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Volume Avg</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Temporale Change</t>
+  </si>
+  <si>
+    <t>Frontal Pole Change</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Change</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Change</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Change</t>
+  </si>
+  <si>
+    <t>Planum Polare Change</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Change</t>
+  </si>
+  <si>
     <t>Central Opercular Cortex Change</t>
   </si>
   <si>
-    <t>Planum Temporale Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Change</t>
-  </si>
-  <si>
-    <t>Insular Cortex Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Change</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Change</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Change</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, superior division Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, anterior division Change</t>
+    <t>Temporal Fusiform Cortex, anterior division Change</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Change</t>
   </si>
   <si>
     <t>Superior Temporal Gyrus, anterior division Change</t>
   </si>
   <si>
-    <t>Temporal Fusiform Cortex, anterior division Change</t>
-  </si>
-  <si>
-    <t>Planum Polare Change</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Change</t>
-  </si>
-  <si>
-    <t>Paracingulate Gyrus Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Change</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Change</t>
-  </si>
-  <si>
-    <t>Occipital Pole Volume Change</t>
+    <t>Occipital Pole Change</t>
   </si>
   <si>
     <t>Cingulate Gyrus, anterior division Change</t>
   </si>
   <si>
+    <t>Frontal Pole Volume Change</t>
+  </si>
+  <si>
     <t>Temporal Pole Change</t>
   </si>
   <si>
-    <t>Lingual Gyrus Change</t>
-  </si>
-  <si>
-    <t>Frontal Medial Cortex Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Paracingulate Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Paracingulate Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, superior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Planum Polare Volume Avg</t>
-  </si>
-  <si>
-    <t>Planum Polare Volume Change</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Change</t>
-  </si>
-  <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Avg</t>
-  </si>
-  <si>
-    <t>Planum Temporale Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Insular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Insular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Temporale Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Volume Avg</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Volume Change</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Volume Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, superior division Volume Change</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Volume Avg</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Change</t>
-  </si>
-  <si>
-    <t>Frontal Pole Change</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Change</t>
-  </si>
-  <si>
-    <t>Occipital Pole Change</t>
+    <t>Temporal Pole Volume Avg</t>
   </si>
   <si>
     <t xml:space="preserve">age at baseline </t>
   </si>
   <si>
-    <t>Occipital Pole Volume Avg</t>
-  </si>
-  <si>
     <t>Supracalcarine Cortex Change</t>
   </si>
   <si>
-    <t>Frontal Medial Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Pole Volume Change</t>
+    <t>Frontal Pole Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, anterior division Volume Change</t>
   </si>
   <si>
     <t>Frontal Medial Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Pole Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Pole Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Pole Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, anterior division Volume Change</t>
   </si>
 </sst>
 </file>
@@ -843,13 +843,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>43.82964001918847</v>
+        <v>35.17363823784722</v>
       </c>
       <c r="C2">
-        <v>0.3617042715652163</v>
+        <v>0.4877625499342637</v>
       </c>
       <c r="D2">
-        <v>0.003882332744808361</v>
+        <v>0.0128025075608416</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -857,13 +857,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>50.27256518816761</v>
+        <v>35.17363823784722</v>
       </c>
       <c r="C3">
-        <v>0.2678752642499862</v>
+        <v>0.4877625499342637</v>
       </c>
       <c r="D3">
-        <v>0.00460519954801258</v>
+        <v>0.0128025075608416</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -871,13 +871,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>51.21334452291418</v>
+        <v>53.75358173131204</v>
       </c>
       <c r="C4">
-        <v>0.2541745943264926</v>
+        <v>0.2171808485731257</v>
       </c>
       <c r="D4">
-        <v>0.004235346921290491</v>
+        <v>0.06667331766110626</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -885,13 +885,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>51.32953773399369</v>
+        <v>54.95752136050536</v>
       </c>
       <c r="C5">
-        <v>0.252482460184558</v>
+        <v>0.1996477471771063</v>
       </c>
       <c r="D5">
-        <v>0.01370050952506687</v>
+        <v>0.01948673835900572</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -899,13 +899,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>51.77270546811044</v>
+        <v>62.40796912650842</v>
       </c>
       <c r="C6">
-        <v>0.2460285611440228</v>
+        <v>0.09114608068191621</v>
       </c>
       <c r="D6">
-        <v>0.007951519736736374</v>
+        <v>0.05214778871355157</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -913,13 +913,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>52.24500947924039</v>
+        <v>62.42597479261672</v>
       </c>
       <c r="C7">
-        <v>0.239150347389703</v>
+        <v>0.0908838622434458</v>
       </c>
       <c r="D7">
-        <v>0.01390325209691019</v>
+        <v>0.07181484117856007</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -927,13 +927,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>52.39111547385767</v>
+        <v>62.47666370091744</v>
       </c>
       <c r="C8">
-        <v>0.2370225901865388</v>
+        <v>0.09014567425848385</v>
       </c>
       <c r="D8">
-        <v>0.02020394565701578</v>
+        <v>0.05985173293516763</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -941,13 +941,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>52.79747503553556</v>
+        <v>63.5157159722098</v>
       </c>
       <c r="C9">
-        <v>0.2311047324922006</v>
+        <v>0.07501384506490572</v>
       </c>
       <c r="D9">
-        <v>0.03156294400790094</v>
+        <v>0.03457142972157175</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -955,13 +955,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>52.84811716862946</v>
+        <v>64.08029480317816</v>
       </c>
       <c r="C10">
-        <v>0.2303672256995709</v>
+        <v>0.06679182325468691</v>
       </c>
       <c r="D10">
-        <v>0.01827745667871282</v>
+        <v>0.06336826509272145</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -969,13 +969,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>53.0462959516558</v>
+        <v>64.45354390145151</v>
       </c>
       <c r="C11">
-        <v>0.227481126917634</v>
+        <v>0.06135615677497797</v>
       </c>
       <c r="D11">
-        <v>0.01837256215316668</v>
+        <v>0.05339066060276446</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -983,13 +983,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>53.24490850081902</v>
+        <v>64.51942528033487</v>
       </c>
       <c r="C12">
-        <v>0.2245887111531212</v>
+        <v>0.06039671921842416</v>
       </c>
       <c r="D12">
-        <v>0.01623753940426115</v>
+        <v>0.06123918375999982</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -997,13 +997,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>54.08759779331723</v>
+        <v>64.61366189745226</v>
       </c>
       <c r="C13">
-        <v>0.2123165369905258</v>
+        <v>0.05902434129923884</v>
       </c>
       <c r="D13">
-        <v>0.00800091219450047</v>
+        <v>0.03745622614157285</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1011,13 +1011,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>54.42247822450501</v>
+        <v>64.76229167147494</v>
       </c>
       <c r="C14">
-        <v>0.2074396375072086</v>
+        <v>0.05685983002706396</v>
       </c>
       <c r="D14">
-        <v>0.01726995635061003</v>
+        <v>0.02407937507585089</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1025,13 +1025,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>54.79309884243684</v>
+        <v>64.81616858165457</v>
       </c>
       <c r="C15">
-        <v>0.2020422498674246</v>
+        <v>0.05607521483027333</v>
       </c>
       <c r="D15">
-        <v>0.01581537858864748</v>
+        <v>0.1117492530952198</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1039,13 +1039,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>55.18175892848411</v>
+        <v>64.86132869326377</v>
       </c>
       <c r="C16">
-        <v>0.1963821515269304</v>
+        <v>0.0554175433019839</v>
       </c>
       <c r="D16">
-        <v>0.02058224528221539</v>
+        <v>0.02474006301050577</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1053,13 +1053,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>55.34022654811989</v>
+        <v>65.03509547823623</v>
       </c>
       <c r="C17">
-        <v>0.1940743706584482</v>
+        <v>0.05288695905481211</v>
       </c>
       <c r="D17">
-        <v>0.01590106009418793</v>
+        <v>0.05894077919525878</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1067,13 +1067,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>55.37393588116091</v>
+        <v>65.23188811179938</v>
       </c>
       <c r="C18">
-        <v>0.193583458041346</v>
+        <v>0.0500210469155431</v>
       </c>
       <c r="D18">
-        <v>0.01535273290715243</v>
+        <v>0.05594776039606391</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1081,13 +1081,13 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>55.47096386607953</v>
+        <v>65.33729617876747</v>
       </c>
       <c r="C19">
-        <v>0.1921704291347642</v>
+        <v>0.04848597797911447</v>
       </c>
       <c r="D19">
-        <v>0.009395484915043028</v>
+        <v>0.09279685370659929</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1095,13 +1095,13 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>55.4757891732641</v>
+        <v>65.87901900720789</v>
       </c>
       <c r="C20">
-        <v>0.1921001576709112</v>
+        <v>0.04059681057464248</v>
       </c>
       <c r="D20">
-        <v>0.01223826059889141</v>
+        <v>0.06229648809335622</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1109,13 +1109,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>55.48553596988729</v>
+        <v>65.95099813137047</v>
       </c>
       <c r="C21">
-        <v>0.1919582140307676</v>
+        <v>0.03954857090237174</v>
       </c>
       <c r="D21">
-        <v>0.008491428474159774</v>
+        <v>0.09215186452455082</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1123,13 +1123,13 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>55.55647117056346</v>
+        <v>66.14737439512821</v>
       </c>
       <c r="C22">
-        <v>0.1909251771277167</v>
+        <v>0.03668872240104559</v>
       </c>
       <c r="D22">
-        <v>0.003358438696923644</v>
+        <v>0.09674025795088334</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1137,13 +1137,13 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>55.8520084537104</v>
+        <v>66.30899208553079</v>
       </c>
       <c r="C23">
-        <v>0.1866212361110134</v>
+        <v>0.03433506671557096</v>
       </c>
       <c r="D23">
-        <v>0.008906301830053651</v>
+        <v>0.0672981908429994</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1151,13 +1151,13 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>55.94262972391375</v>
+        <v>66.41875037562252</v>
       </c>
       <c r="C24">
-        <v>0.1853015088750425</v>
+        <v>0.03273664501520601</v>
       </c>
       <c r="D24">
-        <v>0.01691999994869852</v>
+        <v>0.08528348328444735</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1165,13 +1165,13 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>56.17399873574797</v>
+        <v>66.42815560000894</v>
       </c>
       <c r="C25">
-        <v>0.1819320572463887</v>
+        <v>0.03259967572802525</v>
       </c>
       <c r="D25">
-        <v>0.007273627939610533</v>
+        <v>0.2073706965330712</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1179,13 +1179,13 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>56.24314928982295</v>
+        <v>66.58105419443389</v>
       </c>
       <c r="C26">
-        <v>0.1809250103423842</v>
+        <v>0.03037299716843844</v>
       </c>
       <c r="D26">
-        <v>0.02133519164801764</v>
+        <v>0.02616507334239607</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1193,13 +1193,13 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>57.09232671126805</v>
+        <v>66.73521789702535</v>
       </c>
       <c r="C27">
-        <v>0.1685583488650284</v>
+        <v>0.02812789470351429</v>
       </c>
       <c r="D27">
-        <v>0.01395379724622524</v>
+        <v>0.0768458252692104</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1207,13 +1207,13 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>57.35078205357963</v>
+        <v>66.85144996196557</v>
       </c>
       <c r="C28">
-        <v>0.164794436112918</v>
+        <v>0.02643519472865663</v>
       </c>
       <c r="D28">
-        <v>0.01322562920544901</v>
+        <v>0.02462891134633005</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1221,13 +1221,13 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>57.47217468437834</v>
+        <v>67.10101984387141</v>
       </c>
       <c r="C29">
-        <v>0.1630265822663349</v>
+        <v>0.02280068188536777</v>
       </c>
       <c r="D29">
-        <v>0.01170904274596512</v>
+        <v>0.1069820236736177</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1235,13 +1235,13 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>57.62862815564284</v>
+        <v>67.14690170825364</v>
       </c>
       <c r="C30">
-        <v>0.1607481336556869</v>
+        <v>0.02213249939436457</v>
       </c>
       <c r="D30">
-        <v>0.03452629303765548</v>
+        <v>0.08773344815187537</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1249,13 +1249,13 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>57.67694746897299</v>
+        <v>67.59596926117452</v>
       </c>
       <c r="C31">
-        <v>0.1600444543353449</v>
+        <v>0.01559268066250696</v>
       </c>
       <c r="D31">
-        <v>0.02032190865117174</v>
+        <v>0.07896245573807252</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1263,13 +1263,13 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>57.93972264995686</v>
+        <v>68.02968701177279</v>
       </c>
       <c r="C32">
-        <v>0.1562176313113078</v>
+        <v>0.009276402741172918</v>
       </c>
       <c r="D32">
-        <v>0.04073731721260194</v>
+        <v>0.1330779152921731</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1277,13 +1277,13 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>58.2754881485109</v>
+        <v>68.04584222796689</v>
       </c>
       <c r="C33">
-        <v>0.1513278424974142</v>
+        <v>0.009041132602424007</v>
       </c>
       <c r="D33">
-        <v>0.009237688091861755</v>
+        <v>0.1375134083930428</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1291,13 +1291,13 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>58.65661692333895</v>
+        <v>68.12870810243319</v>
       </c>
       <c r="C34">
-        <v>0.1457774234465201</v>
+        <v>0.007834348022817572</v>
       </c>
       <c r="D34">
-        <v>0.03682842092746497</v>
+        <v>0.1490469071179357</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1305,13 +1305,13 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>59.73198369141307</v>
+        <v>68.34708457582299</v>
       </c>
       <c r="C35">
-        <v>0.1301167423580621</v>
+        <v>0.004654108119082623</v>
       </c>
       <c r="D35">
-        <v>0.02768909672531274</v>
+        <v>0.01935033873469617</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1319,13 +1319,13 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>59.8117319703845</v>
+        <v>68.39168266751079</v>
       </c>
       <c r="C36">
-        <v>0.1289553596545947</v>
+        <v>0.004004621346930137</v>
       </c>
       <c r="D36">
-        <v>0.05384909259798484</v>
+        <v>0.6451025230546796</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1333,13 +1333,13 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>59.91481209692797</v>
+        <v>68.58863643770168</v>
       </c>
       <c r="C37">
-        <v>0.1274541927631849</v>
+        <v>0.001136362557742521</v>
       </c>
       <c r="D37">
-        <v>0.04774671909658303</v>
+        <v>0.03785005886770314</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1347,13 +1347,13 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>60.19689130902832</v>
+        <v>68.59502460597736</v>
       </c>
       <c r="C38">
-        <v>0.1233462430724031</v>
+        <v>0.001043330980912138</v>
       </c>
       <c r="D38">
-        <v>0.02650096610662288</v>
+        <v>0.04363935767524224</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1361,13 +1361,13 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>60.47134657107444</v>
+        <v>68.97404992248943</v>
       </c>
       <c r="C39">
-        <v>0.1193493217804693</v>
+        <v>-0.004476455181884775</v>
       </c>
       <c r="D39">
-        <v>0.01184432518946184</v>
+        <v>0.04914222960021519</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1375,13 +1375,13 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>61.62713368880421</v>
+        <v>68.98946290238379</v>
       </c>
       <c r="C40">
-        <v>0.102517470551395</v>
+        <v>-0.00470091605413292</v>
       </c>
       <c r="D40">
-        <v>0.03634026854406287</v>
+        <v>0.708456534454393</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1389,13 +1389,13 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>62.29698429138788</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C41">
-        <v>0.09276236468852594</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D41">
-        <v>0.1664547747723916</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1403,13 +1403,13 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>62.61172112579162</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C42">
-        <v>0.08817881855643273</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D42">
-        <v>0.015711090886546</v>
+        <v>0.1033608096211918</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1417,13 +1417,13 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>63.54580519146118</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C43">
-        <v>0.07457565255153631</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D43">
-        <v>0.02309120680282317</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1431,13 +1431,13 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>64.71046712749802</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C44">
-        <v>0.05761455639565993</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D44">
-        <v>0.06523224204751547</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1445,13 +1445,13 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>67.36339097623663</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C45">
-        <v>0.01897974306451522</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D45">
-        <v>0.2323104262338641</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1465,7 +1465,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D46">
-        <v>0.02554098979904909</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1479,7 +1479,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D47">
-        <v>0.02554098979904909</v>
+        <v>0.1033608096211916</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1493,7 +1493,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D48">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1507,7 +1507,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D49">
-        <v>0.02554098979904898</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1521,7 +1521,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D50">
-        <v>0.02554098979904919</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1535,7 +1535,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D51">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1563,7 +1563,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D53">
-        <v>0.02554098979904919</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1577,7 +1577,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D54">
-        <v>0.02554098979904909</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1591,7 +1591,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D55">
-        <v>0.02554098979904952</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1605,7 +1605,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D56">
-        <v>0.02554098979904952</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1619,7 +1619,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D57">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1633,7 +1633,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D58">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1647,7 +1647,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D59">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1675,7 +1675,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D61">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1703,7 +1703,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D63">
-        <v>0.02554098979904909</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1717,7 +1717,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D64">
-        <v>0.02554098979904957</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1731,7 +1731,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D65">
-        <v>0.02554098979904909</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1745,7 +1745,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D66">
-        <v>0.02554098979904926</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1759,7 +1759,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D67">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1773,7 +1773,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D68">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1787,7 +1787,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D69">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1801,7 +1801,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D70">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1815,7 +1815,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D71">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1857,7 +1857,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D74">
-        <v>0.02554098979904922</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1871,7 +1871,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D75">
-        <v>0.02554098979904919</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1885,7 +1885,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D76">
-        <v>0.02554098979904944</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1899,7 +1899,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D77">
-        <v>0.02560846533537106</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1913,7 +1913,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D78">
-        <v>0.0256084653353712</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1927,7 +1927,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D79">
-        <v>0.02554098979904923</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1969,7 +1969,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D82">
-        <v>0.02554098979904926</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1983,7 +1983,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D83">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1997,7 +1997,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D84">
-        <v>0.02554098979904909</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2011,7 +2011,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D85">
-        <v>0.0255409897990493</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2025,7 +2025,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D86">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2039,7 +2039,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D87">
-        <v>0.02554098979904932</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2067,7 +2067,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D89">
-        <v>0.02554098979904944</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2081,7 +2081,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D90">
-        <v>0.02554098979905188</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2095,7 +2095,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D91">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2109,7 +2109,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D92">
-        <v>0.02554098979904909</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2123,7 +2123,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D93">
-        <v>0.02554098979904904</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2151,7 +2151,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D95">
-        <v>0.02554098979904926</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2165,7 +2165,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D96">
-        <v>0.02554098979904909</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2179,7 +2179,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D97">
-        <v>0.02554098979904952</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2193,7 +2193,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D98">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2207,7 +2207,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D99">
-        <v>0.02554098979904951</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2221,7 +2221,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D100">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2235,7 +2235,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D101">
-        <v>0.02554098979904937</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2249,7 +2249,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D102">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2263,7 +2263,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D103">
-        <v>0.02554098979904932</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2277,7 +2277,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D104">
-        <v>0.02554098979904948</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2291,7 +2291,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D105">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2305,7 +2305,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D106">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2319,7 +2319,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D107">
-        <v>0.02554098979904962</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2333,7 +2333,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D108">
-        <v>0.02554098979904909</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2347,7 +2347,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D109">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2361,7 +2361,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D110">
-        <v>0.02554098979904909</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2375,7 +2375,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D111">
-        <v>0.02554098979905135</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2389,7 +2389,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D112">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2403,7 +2403,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D113">
-        <v>0.02554098979904948</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2431,7 +2431,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D115">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2445,7 +2445,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D116">
-        <v>0.02554098979904962</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2459,7 +2459,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D117">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2487,7 +2487,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D119">
-        <v>0.02554098979904913</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2501,7 +2501,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D120">
-        <v>0.02554098979904923</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2515,7 +2515,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D121">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2529,7 +2529,7 @@
         <v>-0.008358073230094298</v>
       </c>
       <c r="D122">
-        <v>0.02554098979904942</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2537,13 +2537,13 @@
         <v>125</v>
       </c>
       <c r="B123">
-        <v>69.24058769513314</v>
+        <v>70.11003272513041</v>
       </c>
       <c r="C123">
-        <v>-0.008358073230094298</v>
+        <v>-0.02101989405529725</v>
       </c>
       <c r="D123">
-        <v>0.02554098979904912</v>
+        <v>0.04310898089518717</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2551,13 +2551,13 @@
         <v>126</v>
       </c>
       <c r="B124">
-        <v>69.24058769513314</v>
+        <v>70.68276475702643</v>
       </c>
       <c r="C124">
-        <v>-0.008358073230094298</v>
+        <v>-0.02936065180135583</v>
       </c>
       <c r="D124">
-        <v>0.02554098979904926</v>
+        <v>0.01833102419019689</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2565,13 +2565,13 @@
         <v>127</v>
       </c>
       <c r="B125">
-        <v>69.24058769513314</v>
+        <v>70.75767951386837</v>
       </c>
       <c r="C125">
-        <v>-0.008358073230094298</v>
+        <v>-0.03045164340585016</v>
       </c>
       <c r="D125">
-        <v>0.02554098979904912</v>
+        <v>0.1530145003262824</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2579,13 +2579,13 @@
         <v>128</v>
       </c>
       <c r="B126">
-        <v>69.24058769513314</v>
+        <v>70.88219649252778</v>
       </c>
       <c r="C126">
-        <v>-0.008358073230094298</v>
+        <v>-0.0322649974639968</v>
       </c>
       <c r="D126">
-        <v>0.02554098979904923</v>
+        <v>0.05826485615985685</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2593,13 +2593,13 @@
         <v>129</v>
       </c>
       <c r="B127">
-        <v>69.24058769513314</v>
+        <v>71.23848233614081</v>
       </c>
       <c r="C127">
-        <v>-0.008358073230094298</v>
+        <v>-0.03745362625447779</v>
       </c>
       <c r="D127">
-        <v>0.02554098979904913</v>
+        <v>0.08897873078553088</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2607,13 +2607,13 @@
         <v>130</v>
       </c>
       <c r="B128">
-        <v>69.24374132719311</v>
+        <v>71.29529240718752</v>
       </c>
       <c r="C128">
-        <v>-0.008403999910579163</v>
+        <v>-0.03828095738622594</v>
       </c>
       <c r="D128">
-        <v>0.06377312273760571</v>
+        <v>0.09791436026940799</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2621,13 +2621,13 @@
         <v>131</v>
       </c>
       <c r="B129">
-        <v>69.31515365509853</v>
+        <v>71.34689813444392</v>
       </c>
       <c r="C129">
-        <v>-0.009443985268425159</v>
+        <v>-0.03903249710355228</v>
       </c>
       <c r="D129">
-        <v>0.02298376423891035</v>
+        <v>0.2001384318914233</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2635,13 +2635,13 @@
         <v>132</v>
       </c>
       <c r="B130">
-        <v>70.09793950314105</v>
+        <v>71.35362047882252</v>
       </c>
       <c r="C130">
-        <v>-0.02084377917195712</v>
+        <v>-0.03913039532265805</v>
       </c>
       <c r="D130">
-        <v>0.06632289324755807</v>
+        <v>0.1071624645229187</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2649,13 +2649,13 @@
         <v>133</v>
       </c>
       <c r="B131">
-        <v>75.51812461807199</v>
+        <v>71.38336874235827</v>
       </c>
       <c r="C131">
-        <v>-0.09977851385541725</v>
+        <v>-0.03956362246152811</v>
       </c>
       <c r="D131">
-        <v>0.09518650699452047</v>
+        <v>0.08112442747125795</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2663,13 +2663,13 @@
         <v>134</v>
       </c>
       <c r="B132">
-        <v>78.04832652780568</v>
+        <v>72.88440826268422</v>
       </c>
       <c r="C132">
-        <v>-0.1366261144826071</v>
+        <v>-0.06142342130122658</v>
       </c>
       <c r="D132">
-        <v>0.1993894770059438</v>
+        <v>0.2251565208738294</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2677,13 +2677,13 @@
         <v>135</v>
       </c>
       <c r="B133">
-        <v>82.18647789671594</v>
+        <v>73.5688062211446</v>
       </c>
       <c r="C133">
-        <v>-0.1968904548065429</v>
+        <v>-0.07139038186132907</v>
       </c>
       <c r="D133">
-        <v>0.05506596214507239</v>
+        <v>0.0808335233274166</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2691,13 +2691,13 @@
         <v>136</v>
       </c>
       <c r="B134">
-        <v>83.85911834609003</v>
+        <v>74.27073569996247</v>
       </c>
       <c r="C134">
-        <v>-0.2212492963022819</v>
+        <v>-0.08161265582469635</v>
       </c>
       <c r="D134">
-        <v>0.1300240414387865</v>
+        <v>0.1867529790868659</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2705,13 +2705,13 @@
         <v>137</v>
       </c>
       <c r="B135">
-        <v>129.4975258173286</v>
+        <v>74.77056261512062</v>
       </c>
       <c r="C135">
-        <v>-0.8858862983106111</v>
+        <v>-0.08889168856971796</v>
       </c>
       <c r="D135">
-        <v>0.1318444385279162</v>
+        <v>0.066173901096396</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2719,13 +2719,13 @@
         <v>138</v>
       </c>
       <c r="B136">
-        <v>163.8315736903427</v>
+        <v>77.01222322299694</v>
       </c>
       <c r="C136">
-        <v>-1.385896704228291</v>
+        <v>-0.121537231402868</v>
       </c>
       <c r="D136">
-        <v>0.03010100558100193</v>
+        <v>0.9343795447002573</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2733,13 +2733,13 @@
         <v>139</v>
       </c>
       <c r="B137">
-        <v>166.1277012754091</v>
+        <v>77.32574384477334</v>
       </c>
       <c r="C137">
-        <v>-1.419335455467123</v>
+        <v>-0.1261030657005826</v>
       </c>
       <c r="D137">
-        <v>0.1618111244979356</v>
+        <v>0.1062625749657276</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2747,13 +2747,13 @@
         <v>140</v>
       </c>
       <c r="B138">
-        <v>187.800331913914</v>
+        <v>77.59391276478843</v>
       </c>
       <c r="C138">
-        <v>-1.734956290008455</v>
+        <v>-0.1300084383221616</v>
       </c>
       <c r="D138">
-        <v>0.1518812186638858</v>
+        <v>0.7975571074672535</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2761,13 +2761,13 @@
         <v>141</v>
       </c>
       <c r="B139">
-        <v>324.6058281413501</v>
+        <v>78.04832652780568</v>
       </c>
       <c r="C139">
-        <v>-3.727269341864321</v>
+        <v>-0.1366261144826071</v>
       </c>
       <c r="D139">
-        <v>0.2578024523514668</v>
+        <v>0.1993894770059438</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2775,13 +2775,13 @@
         <v>142</v>
       </c>
       <c r="B140">
-        <v>617.6029945842153</v>
+        <v>82.28569571589868</v>
       </c>
       <c r="C140">
-        <v>-7.994218367731291</v>
+        <v>-0.1983353745033789</v>
       </c>
       <c r="D140">
-        <v>0.03019927070465828</v>
+        <v>0.1779275301750732</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2789,13 +2789,13 @@
         <v>143</v>
       </c>
       <c r="B141">
-        <v>21808.64432629243</v>
+        <v>88.20654028144411</v>
       </c>
       <c r="C141">
-        <v>-316.6016164023169</v>
+        <v>-0.2845612662346229</v>
       </c>
       <c r="D141">
-        <v>0.02427179035916842</v>
+        <v>0.3365725027034847</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2803,13 +2803,13 @@
         <v>144</v>
       </c>
       <c r="B142">
-        <v>25424.30176986883</v>
+        <v>95.25616370808679</v>
       </c>
       <c r="C142">
-        <v>-369.2568218912936</v>
+        <v>-0.3872256850692251</v>
       </c>
       <c r="D142">
-        <v>0.02691530840072508</v>
+        <v>0.1451117273078946</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2817,13 +2817,13 @@
         <v>145</v>
       </c>
       <c r="B143">
-        <v>13807525.38829923</v>
+        <v>95.25616370808683</v>
       </c>
       <c r="C143">
-        <v>-201079.4668198917</v>
+        <v>-0.3872256850692255</v>
       </c>
       <c r="D143">
-        <v>0.02556496413792915</v>
+        <v>0.1451117273078957</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2831,13 +2831,13 @@
         <v>146</v>
       </c>
       <c r="B144">
-        <v>13807525.38829923</v>
+        <v>109.1886935763889</v>
       </c>
       <c r="C144">
-        <v>-201079.4668198917</v>
+        <v>-0.5901266054813916</v>
       </c>
       <c r="D144">
-        <v>0.0255649641379294</v>
+        <v>0.40323571073929</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2845,13 +2845,13 @@
         <v>147</v>
       </c>
       <c r="B145">
-        <v>53705000.61247429</v>
+        <v>109.1886935763889</v>
       </c>
       <c r="C145">
-        <v>-782110.6594049652</v>
+        <v>-0.5901266054813916</v>
       </c>
       <c r="D145">
-        <v>0.02551338187177616</v>
+        <v>0.40323571073929</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2859,13 +2859,13 @@
         <v>148</v>
       </c>
       <c r="B146">
-        <v>53877814.06218128</v>
+        <v>120.4980609304684</v>
       </c>
       <c r="C146">
-        <v>-784627.3601288536</v>
+        <v>-0.7548261300553651</v>
       </c>
       <c r="D146">
-        <v>0.02556864373089735</v>
+        <v>0.5268283171402068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backup: Mon Jan 13 21:28:46 IST 2025
</commit_message>
<xml_diff>
--- a/src/linear_regression_with_significance.xlsx
+++ b/src/linear_regression_with_significance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t>Feature</t>
   </si>
@@ -28,12 +28,6 @@
     <t>Temporal Fusiform Cortex, anterior division Volume Avg</t>
   </si>
   <si>
-    <t>Inferior Temporal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Change</t>
-  </si>
-  <si>
     <t>Middle Temporal Gyrus, posterior division Volume Change</t>
   </si>
   <si>
@@ -106,244 +100,244 @@
     <t>Cingulate Gyrus, posterior division Change</t>
   </si>
   <si>
+    <t>Planum Polare Volume Avg</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Volume Change</t>
+  </si>
+  <si>
     <t>Paracingulate Gyrus Volume Avg</t>
   </si>
   <si>
+    <t>Planum Polare Volume Change</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Change</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Avg</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Volume Change</t>
+  </si>
+  <si>
     <t>Cingulate Gyrus, posterior division Volume Change</t>
   </si>
   <si>
-    <t>Cingulate Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Paracingulate Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Polare Volume Avg</t>
+    <t>Occipital Fusiform Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Insular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Insular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Volume Change</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Volume Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Planum Temporale Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Volume Avg</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Volume Avg</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Temporale Volume Change</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Volume Avg</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Volume Avg</t>
   </si>
   <si>
     <t>Superior Frontal Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Change</t>
-  </si>
-  <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Avg</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Polare Volume Change</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Insular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Insular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Volume Avg</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Planum Temporale Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Planum Temporale Volume Change</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Volume Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Volume Change</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Volume Avg</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, superior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Volume Avg</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, superior division Volume Change</t>
   </si>
   <si>
     <t>Central Opercular Cortex Change</t>
@@ -815,7 +809,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C146"/>
+  <dimension ref="A1:C144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -848,10 +842,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.2817883633112037</v>
+        <v>0.1136376794812413</v>
       </c>
       <c r="C3">
-        <v>0.0128025075608416</v>
+        <v>0.1451117273078946</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -859,10 +853,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1160680805116768</v>
+        <v>0.1136376794812413</v>
       </c>
       <c r="C4">
-        <v>0.01948673835900572</v>
+        <v>0.1451117273078957</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -870,10 +864,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.1136376794812413</v>
+        <v>0.09151606028701342</v>
       </c>
       <c r="C5">
-        <v>0.1451117273078946</v>
+        <v>0.01833102419019689</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -881,10 +875,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.1136376794812413</v>
+        <v>0.07593694587960065</v>
       </c>
       <c r="C6">
-        <v>0.1451117273078957</v>
+        <v>0.07181484117856007</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -892,10 +886,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.09151606028701342</v>
+        <v>0.07224860263943789</v>
       </c>
       <c r="C7">
-        <v>0.01833102419019689</v>
+        <v>0.1117492530952198</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -903,10 +897,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.07593694587960065</v>
+        <v>0.0625782476595963</v>
       </c>
       <c r="C8">
-        <v>0.07181484117856007</v>
+        <v>0.05339066060276446</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -914,10 +908,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0.07224860263943789</v>
+        <v>0.06222407737072744</v>
       </c>
       <c r="C9">
-        <v>0.1117492530952198</v>
+        <v>0.07896245573807252</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -925,10 +919,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.0625782476595963</v>
+        <v>0.0567327407162499</v>
       </c>
       <c r="C10">
-        <v>0.05339066060276446</v>
+        <v>0.09279685370659929</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -936,10 +930,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.06222407737072744</v>
+        <v>0.05175630994285363</v>
       </c>
       <c r="C11">
-        <v>0.07896245573807252</v>
+        <v>0.1069820236736177</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -947,10 +941,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>0.0567327407162499</v>
+        <v>0.05077692433897107</v>
       </c>
       <c r="C12">
-        <v>0.09279685370659929</v>
+        <v>0.1062625749657276</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -958,10 +952,10 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>0.05175630994285363</v>
+        <v>0.0504605473333124</v>
       </c>
       <c r="C13">
-        <v>0.1069820236736177</v>
+        <v>0.09215186452455082</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -969,10 +963,10 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>0.05077692433897107</v>
+        <v>0.04840727405434408</v>
       </c>
       <c r="C14">
-        <v>0.1062625749657276</v>
+        <v>0.03457142972157175</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -980,10 +974,10 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>0.0504605473333124</v>
+        <v>0.04533700282373565</v>
       </c>
       <c r="C15">
-        <v>0.09215186452455082</v>
+        <v>0.0768458252692104</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -991,10 +985,10 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>0.04840727405434408</v>
+        <v>0.03914132458241881</v>
       </c>
       <c r="C16">
-        <v>0.03457142972157175</v>
+        <v>0.08528348328444735</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1002,10 +996,10 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>0.04533700282373565</v>
+        <v>0.03521300698681351</v>
       </c>
       <c r="C17">
-        <v>0.0768458252692104</v>
+        <v>0.1330779152921731</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1013,10 +1007,10 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>0.03914132458241881</v>
+        <v>0.03519996473771236</v>
       </c>
       <c r="C18">
-        <v>0.08528348328444735</v>
+        <v>0.05985173293516763</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1024,10 +1018,10 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>0.03521300698681351</v>
+        <v>0.0337402040453606</v>
       </c>
       <c r="C19">
-        <v>0.1330779152921731</v>
+        <v>0.03745622614157285</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1035,10 +1029,10 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>0.03519996473771236</v>
+        <v>0.02580292165742626</v>
       </c>
       <c r="C20">
-        <v>0.05985173293516763</v>
+        <v>0.2073706965330712</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1046,10 +1040,10 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>0.0337402040453606</v>
+        <v>0.02087641337421142</v>
       </c>
       <c r="C21">
-        <v>0.03745622614157285</v>
+        <v>0.02407937507585089</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1057,10 +1051,10 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>0.02580292165742626</v>
+        <v>0.01690909427152887</v>
       </c>
       <c r="C22">
-        <v>0.2073706965330712</v>
+        <v>0.2251565208738294</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1068,10 +1062,10 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>0.02087641337421142</v>
+        <v>0.008561995176331161</v>
       </c>
       <c r="C23">
-        <v>0.02407937507585089</v>
+        <v>0.06336826509272145</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1079,10 +1073,10 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>0.01690909427152887</v>
+        <v>0.008211841091570582</v>
       </c>
       <c r="C24">
-        <v>0.2251565208738294</v>
+        <v>0.2001384318914233</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1090,10 +1084,10 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>0.008561995176331161</v>
+        <v>-0.001785665108650081</v>
       </c>
       <c r="C25">
-        <v>0.06336826509272145</v>
+        <v>0.08773344815187537</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1101,10 +1095,10 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>0.008211841091570582</v>
+        <v>-0.001814155521589811</v>
       </c>
       <c r="C26">
-        <v>0.2001384318914233</v>
+        <v>0.0672981908429994</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1112,10 +1106,10 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>-0.001785665108650081</v>
+        <v>-0.003048818897637862</v>
       </c>
       <c r="C27">
-        <v>0.08773344815187537</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1123,10 +1117,10 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>-0.001814155521589811</v>
+        <v>-0.003048818897637862</v>
       </c>
       <c r="C28">
-        <v>0.0672981908429994</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1170,7 +1164,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C32">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1181,7 +1175,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C33">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1192,7 +1186,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C34">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1203,7 +1197,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C35">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1214,7 +1208,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C36">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1225,7 +1219,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C37">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1236,7 +1230,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C38">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1247,7 +1241,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C39">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1258,7 +1252,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C40">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1269,7 +1263,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C41">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1291,7 +1285,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C43">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1302,7 +1296,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C44">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1313,7 +1307,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C45">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1324,7 +1318,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C46">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1335,7 +1329,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C47">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1357,7 +1351,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C49">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1445,7 +1439,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C57">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1456,7 +1450,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C58">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1467,7 +1461,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C59">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1500,7 +1494,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C62">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1533,7 +1527,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C65">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1544,7 +1538,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C66">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1555,7 +1549,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C67">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1577,7 +1571,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C69">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1599,7 +1593,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C71">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1643,7 +1637,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C75">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1698,7 +1692,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C80">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1709,7 +1703,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C81">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1720,7 +1714,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C82">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1742,7 +1736,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C84">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1753,7 +1747,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C85">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1819,7 +1813,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C91">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1852,7 +1846,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C94">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1863,7 +1857,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C95">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1929,7 +1923,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C101">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1940,7 +1934,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C102">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1962,7 +1956,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C104">
-        <v>0.02554098979904915</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1973,7 +1967,7 @@
         <v>-0.003048818897637862</v>
       </c>
       <c r="C105">
-        <v>0.02554098979904912</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -1992,10 +1986,10 @@
         <v>108</v>
       </c>
       <c r="B107">
-        <v>-0.003048818897637862</v>
+        <v>-0.01003967456032506</v>
       </c>
       <c r="C107">
-        <v>0.02554098979904912</v>
+        <v>0.1071624645229187</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2003,10 +1997,10 @@
         <v>109</v>
       </c>
       <c r="B108">
-        <v>-0.003048818897637862</v>
+        <v>-0.01108513183959481</v>
       </c>
       <c r="C108">
-        <v>0.02554098979904912</v>
+        <v>0.05894077919525878</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2014,10 +2008,10 @@
         <v>110</v>
       </c>
       <c r="B109">
-        <v>-0.01003967456032506</v>
+        <v>-0.01315282489213576</v>
       </c>
       <c r="C109">
-        <v>0.1071624645229187</v>
+        <v>0.02616507334239607</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2025,10 +2019,10 @@
         <v>111</v>
       </c>
       <c r="B110">
-        <v>-0.01108513183959481</v>
+        <v>-0.01752026602465118</v>
       </c>
       <c r="C110">
-        <v>0.05894077919525878</v>
+        <v>0.708456534454393</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2036,10 +2030,10 @@
         <v>112</v>
       </c>
       <c r="B111">
-        <v>-0.01315282489213576</v>
+        <v>-0.02000755648054064</v>
       </c>
       <c r="C111">
-        <v>0.02616507334239607</v>
+        <v>0.03785005886770314</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2047,10 +2041,10 @@
         <v>113</v>
       </c>
       <c r="B112">
-        <v>-0.01752026602465118</v>
+        <v>-0.02329678625712317</v>
       </c>
       <c r="C112">
-        <v>0.708456534454393</v>
+        <v>0.02462891134633005</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2058,10 +2052,10 @@
         <v>114</v>
       </c>
       <c r="B113">
-        <v>-0.02000755648054064</v>
+        <v>-0.02547640729626655</v>
       </c>
       <c r="C113">
-        <v>0.03785005886770314</v>
+        <v>0.06123918375999982</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2069,10 +2063,10 @@
         <v>115</v>
       </c>
       <c r="B114">
-        <v>-0.02329678625712317</v>
+        <v>-0.02640970388949415</v>
       </c>
       <c r="C114">
-        <v>0.02462891134633005</v>
+        <v>0.08112442747125795</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2080,10 +2074,10 @@
         <v>116</v>
       </c>
       <c r="B115">
-        <v>-0.02547640729626655</v>
+        <v>-0.03567736011137357</v>
       </c>
       <c r="C115">
-        <v>0.06123918375999982</v>
+        <v>0.05594776039606391</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2091,10 +2085,10 @@
         <v>117</v>
       </c>
       <c r="B116">
-        <v>-0.02640970388949415</v>
+        <v>-0.03617535841328912</v>
       </c>
       <c r="C116">
-        <v>0.08112442747125795</v>
+        <v>0.02474006301050577</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2102,10 +2096,10 @@
         <v>118</v>
       </c>
       <c r="B117">
-        <v>-0.03567736011137357</v>
+        <v>-0.04205226695020814</v>
       </c>
       <c r="C117">
-        <v>0.05594776039606391</v>
+        <v>0.09791436026940799</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2113,10 +2107,10 @@
         <v>119</v>
       </c>
       <c r="B118">
-        <v>-0.03617535841328912</v>
+        <v>-0.04330078586772768</v>
       </c>
       <c r="C118">
-        <v>0.02474006301050577</v>
+        <v>0.1530145003262824</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2124,10 +2118,10 @@
         <v>120</v>
       </c>
       <c r="B119">
-        <v>-0.04205226695020814</v>
+        <v>-0.04786691683353195</v>
       </c>
       <c r="C119">
-        <v>0.09791436026940799</v>
+        <v>0.09674025795088334</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2135,10 +2129,10 @@
         <v>121</v>
       </c>
       <c r="B120">
-        <v>-0.04330078586772768</v>
+        <v>-0.04995671560907833</v>
       </c>
       <c r="C120">
-        <v>0.1530145003262824</v>
+        <v>0.1375134083930428</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2146,10 +2140,10 @@
         <v>122</v>
       </c>
       <c r="B121">
-        <v>-0.04786691683353195</v>
+        <v>-0.05721000431594758</v>
       </c>
       <c r="C121">
-        <v>0.09674025795088334</v>
+        <v>0.1993894770059438</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2157,10 +2151,10 @@
         <v>123</v>
       </c>
       <c r="B122">
-        <v>-0.04995671560907833</v>
+        <v>-0.05892552099498194</v>
       </c>
       <c r="C122">
-        <v>0.1375134083930428</v>
+        <v>0.04914222960021519</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2168,10 +2162,10 @@
         <v>124</v>
       </c>
       <c r="B123">
-        <v>-0.05721000431594758</v>
+        <v>-0.06388677987849789</v>
       </c>
       <c r="C123">
-        <v>0.1993894770059438</v>
+        <v>0.01935033873469617</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2179,10 +2173,10 @@
         <v>125</v>
       </c>
       <c r="B124">
-        <v>-0.05892552099498194</v>
+        <v>-0.06579752361764402</v>
       </c>
       <c r="C124">
-        <v>0.04914222960021519</v>
+        <v>0.05214778871355157</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2190,10 +2184,10 @@
         <v>126</v>
       </c>
       <c r="B125">
-        <v>-0.06388677987849789</v>
+        <v>-0.06951675410818781</v>
       </c>
       <c r="C125">
-        <v>0.01935033873469617</v>
+        <v>0.06229648809335622</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2201,10 +2195,10 @@
         <v>127</v>
       </c>
       <c r="B126">
-        <v>-0.06579752361764402</v>
+        <v>-0.07782916466843837</v>
       </c>
       <c r="C126">
-        <v>0.05214778871355157</v>
+        <v>0.06667331766110626</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2212,10 +2206,10 @@
         <v>128</v>
       </c>
       <c r="B127">
-        <v>-0.06951675410818781</v>
+        <v>-0.09123503176784054</v>
       </c>
       <c r="C127">
-        <v>0.06229648809335622</v>
+        <v>0.7975571074672535</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2223,10 +2217,10 @@
         <v>129</v>
       </c>
       <c r="B128">
-        <v>-0.07782916466843837</v>
+        <v>-0.09185218128229922</v>
       </c>
       <c r="C128">
-        <v>0.06667331766110626</v>
+        <v>0.08897873078553088</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2234,10 +2228,10 @@
         <v>130</v>
       </c>
       <c r="B129">
-        <v>-0.09123503176784054</v>
+        <v>-0.09992060018012072</v>
       </c>
       <c r="C129">
-        <v>0.7975571074672535</v>
+        <v>0.6451025230546796</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2245,10 +2239,10 @@
         <v>131</v>
       </c>
       <c r="B130">
-        <v>-0.09185218128229922</v>
+        <v>-0.1027221353755776</v>
       </c>
       <c r="C130">
-        <v>0.08897873078553088</v>
+        <v>0.066173901096396</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2256,10 +2250,10 @@
         <v>132</v>
       </c>
       <c r="B131">
-        <v>-0.09992060018012072</v>
+        <v>-0.1032391808421085</v>
       </c>
       <c r="C131">
-        <v>0.6451025230546796</v>
+        <v>0.04363935767524224</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2267,10 +2261,10 @@
         <v>133</v>
       </c>
       <c r="B132">
-        <v>-0.1027221353755776</v>
+        <v>-0.1036264067135135</v>
       </c>
       <c r="C132">
-        <v>0.066173901096396</v>
+        <v>0.04310898089518717</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2278,10 +2272,10 @@
         <v>134</v>
       </c>
       <c r="B133">
-        <v>-0.1032391808421085</v>
+        <v>-0.1135178516885138</v>
       </c>
       <c r="C133">
-        <v>0.04363935767524224</v>
+        <v>0.0808335233274166</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2289,10 +2283,10 @@
         <v>135</v>
       </c>
       <c r="B134">
-        <v>-0.1036264067135135</v>
+        <v>-0.1184037501275577</v>
       </c>
       <c r="C134">
-        <v>0.04310898089518717</v>
+        <v>0.1779275301750732</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2300,10 +2294,10 @@
         <v>136</v>
       </c>
       <c r="B135">
-        <v>-0.1135178516885138</v>
+        <v>-0.1320793725494485</v>
       </c>
       <c r="C135">
-        <v>0.0808335233274166</v>
+        <v>0.05826485615985685</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2311,10 +2305,10 @@
         <v>137</v>
       </c>
       <c r="B136">
-        <v>-0.1184037501275577</v>
+        <v>-0.1345607950863972</v>
       </c>
       <c r="C136">
-        <v>0.1779275301750732</v>
+        <v>0.9343795447002573</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2322,10 +2316,10 @@
         <v>138</v>
       </c>
       <c r="B137">
-        <v>-0.1320793725494485</v>
+        <v>-0.1388947166391119</v>
       </c>
       <c r="C137">
-        <v>0.05826485615985685</v>
+        <v>0.1867529790868659</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2333,10 +2327,10 @@
         <v>139</v>
       </c>
       <c r="B138">
-        <v>-0.1345607950863972</v>
+        <v>-0.1954141043440032</v>
       </c>
       <c r="C138">
-        <v>0.9343795447002573</v>
+        <v>0.1490469071179357</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2344,10 +2338,10 @@
         <v>140</v>
       </c>
       <c r="B139">
-        <v>-0.1388947166391119</v>
+        <v>-0.3450366038803971</v>
       </c>
       <c r="C139">
-        <v>0.1867529790868659</v>
+        <v>0.40323571073929</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2355,10 +2349,10 @@
         <v>141</v>
       </c>
       <c r="B140">
-        <v>-0.1954141043440032</v>
+        <v>-0.3450366038803971</v>
       </c>
       <c r="C140">
-        <v>0.1490469071179357</v>
+        <v>0.40323571073929</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2366,10 +2360,10 @@
         <v>142</v>
       </c>
       <c r="B141">
-        <v>-0.3450366038803971</v>
+        <v>-0.3497400638411252</v>
       </c>
       <c r="C141">
-        <v>0.40323571073929</v>
+        <v>0.3365725027034847</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2377,10 +2371,10 @@
         <v>143</v>
       </c>
       <c r="B142">
-        <v>-0.3450366038803971</v>
+        <v>-0.5502294175544231</v>
       </c>
       <c r="C142">
-        <v>0.40323571073929</v>
+        <v>0.1033608096211918</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2388,10 +2382,10 @@
         <v>144</v>
       </c>
       <c r="B143">
-        <v>-0.3497400638411252</v>
+        <v>-0.5502294175544231</v>
       </c>
       <c r="C143">
-        <v>0.3365725027034847</v>
+        <v>0.1033608096211916</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2399,31 +2393,9 @@
         <v>145</v>
       </c>
       <c r="B144">
-        <v>-0.5502294175544231</v>
+        <v>-0.6194609953167622</v>
       </c>
       <c r="C144">
-        <v>0.1033608096211918</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="A145" t="s">
-        <v>146</v>
-      </c>
-      <c r="B145">
-        <v>-0.5502294175544231</v>
-      </c>
-      <c r="C145">
-        <v>0.1033608096211916</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3">
-      <c r="A146" t="s">
-        <v>147</v>
-      </c>
-      <c r="B146">
-        <v>-0.6194609953167622</v>
-      </c>
-      <c r="C146">
         <v>0.5268283171402068</v>
       </c>
     </row>

</xml_diff>